<commit_message>
Fix Google sign-in: Switch from popup to redirect method for better compatibility
</commit_message>
<xml_diff>
--- a/src/bookings/all-bookings.xlsx
+++ b/src/bookings/all-bookings.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Booking ID</t>
   </si>
@@ -113,6 +113,21 @@
   </si>
   <si>
     <t>4/17/2025, 10:15:47 PM</t>
+  </si>
+  <si>
+    <t>2025-04-18T08-52-52-064Z</t>
+  </si>
+  <si>
+    <t>kamal</t>
+  </si>
+  <si>
+    <t>6729738922</t>
+  </si>
+  <si>
+    <t>03:00 PM - 04:00 PM</t>
+  </si>
+  <si>
+    <t>4/18/2025, 2:22:52 PM</t>
   </si>
 </sst>
 </file>
@@ -504,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -646,6 +661,32 @@
         <v>33</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>